<commit_message>
Scheduler now considers school preference
</commit_message>
<xml_diff>
--- a/Input_Specification.xlsx
+++ b/Input_Specification.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15040" tabRatio="500"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="14060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -72,9 +72,6 @@
     <t>YES/NO</t>
   </si>
   <si>
-    <t>teacher_preference</t>
-  </si>
-  <si>
     <t>teacher_email</t>
   </si>
   <si>
@@ -157,6 +154,9 @@
   </si>
   <si>
     <t>Thanks so much!</t>
+  </si>
+  <si>
+    <t>school_preference</t>
   </si>
 </sst>
 </file>
@@ -631,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -679,28 +679,28 @@
         <v>4</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="16">
@@ -732,7 +732,7 @@
         <v>16</v>
       </c>
       <c r="J3" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>15</v>
@@ -740,49 +740,49 @@
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
         <v>28</v>
       </c>
-      <c r="B4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" t="s">
-        <v>29</v>
-      </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -792,7 +792,7 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>2</v>
@@ -801,63 +801,63 @@
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K6" s="1" t="s">
+      <c r="M6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M6" s="1" t="s">
+      <c r="O6" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="16">
       <c r="A7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
         <v>32</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>33</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>34</v>
       </c>
-      <c r="D7" t="s">
-        <v>35</v>
-      </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F7">
         <v>5</v>
       </c>
       <c r="G7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H7">
         <v>2</v>
@@ -866,57 +866,57 @@
         <v>4</v>
       </c>
       <c r="J7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" t="s">
         <v>28</v>
       </c>
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" t="s">
-        <v>29</v>
-      </c>
       <c r="G8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Input Spec. Generated a single-file executable. Packaged Scheduler up for Madison House with included README
</commit_message>
<xml_diff>
--- a/Input_Specification.xlsx
+++ b/Input_Specification.xlsx
@@ -147,9 +147,6 @@
     <t>number (put 0 if you want to go alone)</t>
   </si>
   <si>
-    <t>string (teacher may specify a collection of hour-long openings; if time intervals are allowed to overlap, they may get overlapping helpers.)</t>
-  </si>
-  <si>
     <t>special_msg</t>
   </si>
   <si>
@@ -157,6 +154,9 @@
   </si>
   <si>
     <t>school_preference</t>
+  </si>
+  <si>
+    <t>string (teachers may specify a collection of hour-long openings)</t>
   </si>
 </sst>
 </file>
@@ -631,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -685,7 +685,7 @@
         <v>5</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>22</v>
@@ -819,7 +819,7 @@
         <v>20</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>22</v>
@@ -866,7 +866,7 @@
         <v>4</v>
       </c>
       <c r="J7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>37</v>
@@ -904,7 +904,7 @@
         <v>27</v>
       </c>
       <c r="K8" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="L8" t="s">
         <v>27</v>

</xml_diff>